<commit_message>
Cronograma de Setembro Individual
</commit_message>
<xml_diff>
--- a/Orientador/Cronograma de Trabalho.xlsx
+++ b/Orientador/Cronograma de Trabalho.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eduardo\Dropbox\Documentos\FSARENA\TCC\SrMartis\Orientador\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9327417A-F962-40D5-96AD-EE14FA0288AB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{169747B2-86F2-4F91-9D3E-6681E71302E0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F8E67894-4B5D-4F9E-A861-718F3945718C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{F8E67894-4B5D-4F9E-A861-718F3945718C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="GERAL" sheetId="1" r:id="rId1"/>
+    <sheet name="INDIVIDUAL" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="56">
   <si>
     <t xml:space="preserve">TCC - OTIMIZAÇÃO DE PROCESSOS EM REFEITÓRIO </t>
   </si>
@@ -190,12 +191,45 @@
   <si>
     <t>Pesquisa - elaboração - revisão da pesquisa</t>
   </si>
+  <si>
+    <t>Igor Martins Ferreira</t>
+  </si>
+  <si>
+    <t>Ranan Dias de Oliveira</t>
+  </si>
+  <si>
+    <t>Setembro</t>
+  </si>
+  <si>
+    <t>Outubro</t>
+  </si>
+  <si>
+    <t>Novembro</t>
+  </si>
+  <si>
+    <t>Resenha pelo menos de 2 ARTIGOS sobre IA e Machine Learning</t>
+  </si>
+  <si>
+    <t>Resenha pelo menos de 2 ARTIGOS sobre Definição de disperdício(qualitativo ou quantitativo).</t>
+  </si>
+  <si>
+    <t>Resenha pelo menos de 2 ARTIGOS sobre Metodologias e abordagens para redução do disperdício.</t>
+  </si>
+  <si>
+    <t>TODOS</t>
+  </si>
+  <si>
+    <t>Formalização dos Itens 2, 3, 4, 5 e 6 relativos aos itens que devem ser entregues</t>
+  </si>
+  <si>
+    <t>Mês/Alunos</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -267,8 +301,21 @@
       <name val="Verdana"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -296,6 +343,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -327,70 +392,90 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="10" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -708,8 +793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E1957A1-3A14-45CE-B57F-02189A101F25}">
   <dimension ref="A1:B66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -718,530 +803,611 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
+      <c r="B1" s="20"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
+      <c r="B2" s="21"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
+      <c r="A4" s="2">
         <v>43682</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="4">
+      <c r="A5" s="2">
         <v>43683</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="4">
+      <c r="A6" s="2">
         <v>43689</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="4">
+      <c r="A7" s="2">
         <v>43690</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="4">
+      <c r="A8" s="2">
         <v>43696</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="4">
+      <c r="A9" s="2">
         <v>43697</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="7">
+      <c r="A10" s="5">
         <v>43703</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="4">
+      <c r="A11" s="2">
         <v>43704</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="9">
+      <c r="A12" s="7">
         <v>43707</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="2"/>
+      <c r="B13" s="21"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="7">
+      <c r="A15" s="5">
         <v>43710</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="9" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="4">
+      <c r="A16" s="2">
         <v>43711</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="10" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="51.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="9">
+      <c r="A17" s="7">
         <v>43714</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="11" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="4">
+      <c r="A18" s="2">
         <v>43717</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="10" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="4">
+      <c r="A19" s="2">
         <v>43718</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="10" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="39" x14ac:dyDescent="0.3">
-      <c r="A20" s="9">
+      <c r="A20" s="7">
         <v>43721</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="11" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="4">
+      <c r="A21" s="2">
         <v>43724</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="10" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="4">
+      <c r="A22" s="2">
         <v>43725</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="10" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A23" s="9">
+      <c r="A23" s="7">
         <v>43728</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="12" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="4">
+      <c r="A24" s="2">
         <v>43731</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="7">
+      <c r="A25" s="5">
         <v>43732</v>
       </c>
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="9" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="15">
+      <c r="A26" s="13">
         <v>43735</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="7">
+      <c r="A27" s="5">
         <v>43738</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="9" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="2"/>
+      <c r="B28" s="21"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="4">
+      <c r="A30" s="2">
         <v>43739</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A31" s="9">
+      <c r="A31" s="7">
         <v>43742</v>
       </c>
-      <c r="B31" s="13" t="s">
+      <c r="B31" s="11" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="4">
+      <c r="A32" s="2">
         <v>43745</v>
       </c>
-      <c r="B32" s="12" t="s">
+      <c r="B32" s="10" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="4">
+      <c r="A33" s="2">
         <v>43746</v>
       </c>
-      <c r="B33" s="12" t="s">
+      <c r="B33" s="10" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="39" x14ac:dyDescent="0.3">
-      <c r="A34" s="9">
+      <c r="A34" s="7">
         <v>43749</v>
       </c>
-      <c r="B34" s="13" t="s">
+      <c r="B34" s="11" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="4">
+      <c r="A35" s="2">
         <v>43752</v>
       </c>
-      <c r="B35" s="12" t="s">
+      <c r="B35" s="10" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" s="4">
+      <c r="A36" s="2">
         <v>43753</v>
       </c>
-      <c r="B36" s="12" t="s">
+      <c r="B36" s="10" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="39" x14ac:dyDescent="0.3">
-      <c r="A37" s="9">
+      <c r="A37" s="7">
         <v>43756</v>
       </c>
-      <c r="B37" s="13" t="s">
+      <c r="B37" s="11" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" s="4">
+      <c r="A38" s="2">
         <v>43759</v>
       </c>
-      <c r="B38" s="12" t="s">
+      <c r="B38" s="10" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" s="4">
+      <c r="A39" s="2">
         <v>43760</v>
       </c>
-      <c r="B39" s="12" t="s">
+      <c r="B39" s="10" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="39" x14ac:dyDescent="0.3">
-      <c r="A40" s="16">
+      <c r="A40" s="14">
         <v>43756</v>
       </c>
-      <c r="B40" s="13" t="s">
+      <c r="B40" s="11" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" s="4">
+      <c r="A41" s="2">
         <v>43763</v>
       </c>
-      <c r="B41" s="12" t="s">
+      <c r="B41" s="10" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" s="4">
+      <c r="A42" s="2">
         <v>43767</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B42" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" s="2" t="s">
+      <c r="A43" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="B43" s="2"/>
+      <c r="B43" s="21"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" s="3" t="s">
+      <c r="A44" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B44" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" s="9">
+      <c r="A45" s="7">
         <v>43770</v>
       </c>
-      <c r="B45" s="14" t="s">
+      <c r="B45" s="12" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" s="17">
+      <c r="A46" s="15">
         <v>43773</v>
       </c>
-      <c r="B46" s="11" t="s">
+      <c r="B46" s="9" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" s="4">
+      <c r="A47" s="2">
         <v>43774</v>
       </c>
-      <c r="B47" s="12" t="s">
+      <c r="B47" s="10" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="39" x14ac:dyDescent="0.3">
-      <c r="A48" s="18">
+      <c r="A48" s="16">
         <v>43777</v>
       </c>
-      <c r="B48" s="13" t="s">
+      <c r="B48" s="11" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" s="4">
+      <c r="A49" s="2">
         <v>43780</v>
       </c>
-      <c r="B49" s="12" t="s">
+      <c r="B49" s="10" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50" s="4">
+      <c r="A50" s="2">
         <v>43781</v>
       </c>
-      <c r="B50" s="12" t="s">
+      <c r="B50" s="10" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51" s="19">
+      <c r="A51" s="17">
         <v>43784</v>
       </c>
-      <c r="B51" s="20" t="s">
+      <c r="B51" s="18" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A52" s="4">
+      <c r="A52" s="2">
         <v>43787</v>
       </c>
-      <c r="B52" s="12" t="s">
+      <c r="B52" s="10" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A53" s="4">
+      <c r="A53" s="2">
         <v>43788</v>
       </c>
-      <c r="B53" s="12" t="s">
+      <c r="B53" s="10" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A54" s="18">
+      <c r="A54" s="16">
         <v>43791</v>
       </c>
-      <c r="B54" s="13" t="s">
+      <c r="B54" s="11" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A55" s="4">
+      <c r="A55" s="2">
         <v>43794</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B55" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A56" s="7">
+      <c r="A56" s="5">
         <v>43795</v>
       </c>
-      <c r="B56" s="21" t="s">
+      <c r="B56" s="19" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A57" s="18">
+      <c r="A57" s="16">
         <v>43798</v>
       </c>
-      <c r="B57" s="14" t="s">
+      <c r="B57" s="12" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A58" s="2" t="s">
+      <c r="A58" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="B58" s="2"/>
+      <c r="B58" s="21"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A59" s="7">
+      <c r="A59" s="5">
         <v>43801</v>
       </c>
-      <c r="B59" s="11" t="s">
+      <c r="B59" s="9" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A60" s="4">
+      <c r="A60" s="2">
         <v>43802</v>
       </c>
-      <c r="B60" s="12" t="s">
+      <c r="B60" s="10" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="39" x14ac:dyDescent="0.3">
-      <c r="A61" s="9">
+      <c r="A61" s="7">
         <v>43805</v>
       </c>
-      <c r="B61" s="13" t="s">
+      <c r="B61" s="11" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A62" s="4">
+      <c r="A62" s="2">
         <v>43808</v>
       </c>
-      <c r="B62" s="12" t="s">
+      <c r="B62" s="10" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A63" s="4">
+      <c r="A63" s="2">
         <v>43809</v>
       </c>
-      <c r="B63" s="12" t="s">
+      <c r="B63" s="10" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="39" x14ac:dyDescent="0.3">
-      <c r="A64" s="9">
+      <c r="A64" s="7">
         <v>43812</v>
       </c>
-      <c r="B64" s="13" t="s">
+      <c r="B64" s="11" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A65" s="4">
+      <c r="A65" s="2">
         <v>43815</v>
       </c>
-      <c r="B65" s="12" t="s">
+      <c r="B65" s="10" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A66" s="4">
+      <c r="A66" s="2">
         <v>43816</v>
       </c>
-      <c r="B66" s="12" t="s">
+      <c r="B66" s="10" t="s">
         <v>44</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A58:B58"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A58:B58"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6991E9C-2B49-4914-A2F8-9F7A70301DF8}">
+  <dimension ref="A2:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.5546875" style="22" customWidth="1"/>
+    <col min="2" max="2" width="31.88671875" style="22" customWidth="1"/>
+    <col min="3" max="3" width="33.33203125" style="22" customWidth="1"/>
+    <col min="4" max="4" width="32.109375" style="22" customWidth="1"/>
+    <col min="5" max="5" width="22.5546875" style="22" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="22"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="31" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="28"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="24"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="28"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="24"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>